<commit_message>
0.0.8: if first element of array is '[]', the array's elements are ignored and empty array is set as value.
</commit_message>
<xml_diff>
--- a/meta/test/03_GetTableSample4.xlsx
+++ b/meta/test/03_GetTableSample4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6341C35E-AB6A-354E-BE34-5D6800007C16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839133DB-BAFB-5145-8747-D48643DDDD25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19000" yWindow="3740" windowWidth="26200" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12200" yWindow="3740" windowWidth="26200" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="116">
   <si>
     <t>2.定義書様式に記入された情報から、メタファイルをXMLファイルに変換する処理の定義に相当するJavaソースコードが自動生成されます。</t>
   </si>
@@ -623,6 +623,10 @@
   </si>
   <si>
     <t>reason[]</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>[]</t>
     <phoneticPr fontId="12"/>
   </si>
 </sst>
@@ -2621,6 +2625,72 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="91" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="92" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="93" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="76" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="94" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="83" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="95" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="97" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2638,72 +2708,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="91" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="92" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="93" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="76" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="94" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="83" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="95" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="97" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -3282,20 +3286,20 @@
       <c r="J19" s="140"/>
       <c r="K19" s="140"/>
       <c r="L19" s="141"/>
-      <c r="M19" s="189" t="s">
+      <c r="M19" s="211" t="s">
         <v>43</v>
       </c>
-      <c r="N19" s="190"/>
-      <c r="O19" s="190"/>
-      <c r="P19" s="190"/>
-      <c r="Q19" s="190"/>
-      <c r="R19" s="189" t="s">
+      <c r="N19" s="212"/>
+      <c r="O19" s="212"/>
+      <c r="P19" s="212"/>
+      <c r="Q19" s="212"/>
+      <c r="R19" s="211" t="s">
         <v>44</v>
       </c>
-      <c r="S19" s="190"/>
-      <c r="T19" s="190"/>
-      <c r="U19" s="190"/>
-      <c r="V19" s="190"/>
+      <c r="S19" s="212"/>
+      <c r="T19" s="212"/>
+      <c r="U19" s="212"/>
+      <c r="V19" s="212"/>
       <c r="W19" s="142"/>
     </row>
     <row r="20" spans="1:23" ht="12.75" customHeight="1">
@@ -3313,20 +3317,20 @@
       <c r="J20" s="117"/>
       <c r="K20" s="117"/>
       <c r="L20" s="143"/>
-      <c r="M20" s="187" t="s">
+      <c r="M20" s="209" t="s">
         <v>66</v>
       </c>
-      <c r="N20" s="188"/>
-      <c r="O20" s="188"/>
-      <c r="P20" s="188"/>
-      <c r="Q20" s="188"/>
-      <c r="R20" s="187" t="s">
+      <c r="N20" s="210"/>
+      <c r="O20" s="210"/>
+      <c r="P20" s="210"/>
+      <c r="Q20" s="210"/>
+      <c r="R20" s="209" t="s">
         <v>66</v>
       </c>
-      <c r="S20" s="188"/>
-      <c r="T20" s="188"/>
-      <c r="U20" s="188"/>
-      <c r="V20" s="188"/>
+      <c r="S20" s="210"/>
+      <c r="T20" s="210"/>
+      <c r="U20" s="210"/>
+      <c r="V20" s="210"/>
       <c r="W20" s="117"/>
     </row>
     <row r="21" spans="1:23" ht="23" customHeight="1">
@@ -5766,8 +5770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2255131-13B1-484A-9393-AFEFC966B3D8}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -5931,13 +5935,13 @@
       <c r="D13" s="165" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="191" t="s">
+      <c r="E13" s="213" t="s">
         <v>85</v>
       </c>
-      <c r="F13" s="192"/>
-      <c r="G13" s="192"/>
-      <c r="H13" s="192"/>
-      <c r="I13" s="192"/>
+      <c r="F13" s="214"/>
+      <c r="G13" s="214"/>
+      <c r="H13" s="214"/>
+      <c r="I13" s="214"/>
     </row>
     <row r="14" spans="1:9" s="169" customFormat="1" ht="15" thickBot="1">
       <c r="A14" s="166">
@@ -5975,19 +5979,19 @@
       </c>
       <c r="C15" s="173"/>
       <c r="D15" s="173"/>
-      <c r="E15" s="193" t="s">
+      <c r="E15" s="187" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="194" t="s">
+      <c r="F15" s="188" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="194" t="s">
+      <c r="G15" s="188" t="s">
         <v>87</v>
       </c>
-      <c r="H15" s="195" t="s">
+      <c r="H15" s="189" t="s">
         <v>87</v>
       </c>
-      <c r="I15" s="196" t="s">
+      <c r="I15" s="190" t="s">
         <v>87</v>
       </c>
     </row>
@@ -6012,10 +6016,10 @@
       <c r="G16" s="174" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="197" t="s">
+      <c r="H16" s="191" t="s">
         <v>99</v>
       </c>
-      <c r="I16" s="198" t="s">
+      <c r="I16" s="192" t="s">
         <v>100</v>
       </c>
     </row>
@@ -6040,10 +6044,10 @@
       <c r="G17" s="174" t="s">
         <v>91</v>
       </c>
-      <c r="H17" s="197" t="s">
+      <c r="H17" s="191" t="s">
         <v>99</v>
       </c>
-      <c r="I17" s="198"/>
+      <c r="I17" s="192"/>
     </row>
     <row r="18" spans="1:10" s="169" customFormat="1">
       <c r="A18" s="166">
@@ -6066,10 +6070,10 @@
       <c r="G18" s="174" t="s">
         <v>105</v>
       </c>
-      <c r="H18" s="197" t="s">
+      <c r="H18" s="191" t="s">
         <v>106</v>
       </c>
-      <c r="I18" s="198" t="s">
+      <c r="I18" s="192" t="s">
         <v>107</v>
       </c>
     </row>
@@ -6088,8 +6092,8 @@
       <c r="G19" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="H19" s="199"/>
-      <c r="I19" s="200"/>
+      <c r="H19" s="193"/>
+      <c r="I19" s="194"/>
     </row>
     <row r="20" spans="1:10" s="169" customFormat="1" ht="15" thickBot="1">
       <c r="A20" s="166">
@@ -6104,12 +6108,12 @@
       <c r="E20" s="179" t="s">
         <v>90</v>
       </c>
-      <c r="F20" s="201"/>
-      <c r="G20" s="202" t="s">
+      <c r="F20" s="195"/>
+      <c r="G20" s="196" t="s">
         <v>91</v>
       </c>
-      <c r="H20" s="203"/>
-      <c r="I20" s="204"/>
+      <c r="H20" s="197"/>
+      <c r="I20" s="198"/>
     </row>
     <row r="21" spans="1:10" s="169" customFormat="1">
       <c r="A21" s="166">
@@ -6121,19 +6125,19 @@
       </c>
       <c r="C21" s="173"/>
       <c r="D21" s="173"/>
-      <c r="E21" s="193" t="s">
+      <c r="E21" s="187" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="194" t="s">
+      <c r="F21" s="188" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="194" t="s">
+      <c r="G21" s="188" t="s">
         <v>87</v>
       </c>
-      <c r="H21" s="195" t="s">
+      <c r="H21" s="189" t="s">
         <v>87</v>
       </c>
-      <c r="I21" s="196" t="s">
+      <c r="I21" s="190" t="s">
         <v>87</v>
       </c>
     </row>
@@ -6148,7 +6152,7 @@
       <c r="C22" s="168" t="s">
         <v>109</v>
       </c>
-      <c r="D22" s="205" t="s">
+      <c r="D22" s="199" t="s">
         <v>110</v>
       </c>
       <c r="E22" s="178" t="s">
@@ -6156,10 +6160,10 @@
       </c>
       <c r="F22" s="174"/>
       <c r="G22" s="174"/>
-      <c r="H22" s="197" t="s">
+      <c r="H22" s="191" t="s">
         <v>99</v>
       </c>
-      <c r="I22" s="198" t="s">
+      <c r="I22" s="192" t="s">
         <v>100</v>
       </c>
       <c r="J22" s="176"/>
@@ -6173,7 +6177,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="170"/>
-      <c r="D23" s="200" t="s">
+      <c r="D23" s="194" t="s">
         <v>63</v>
       </c>
       <c r="E23" s="175"/>
@@ -6181,8 +6185,8 @@
       <c r="G23" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="H23" s="199"/>
-      <c r="I23" s="200"/>
+      <c r="H23" s="193"/>
+      <c r="I23" s="194"/>
       <c r="J23" s="176"/>
     </row>
     <row r="24" spans="1:10" s="169" customFormat="1">
@@ -6194,18 +6198,20 @@
         <v>62</v>
       </c>
       <c r="C24" s="170"/>
-      <c r="D24" s="206"/>
+      <c r="D24" s="200"/>
       <c r="E24" s="178" t="s">
         <v>101</v>
       </c>
       <c r="F24" s="174" t="s">
         <v>102</v>
       </c>
-      <c r="G24" s="174"/>
-      <c r="H24" s="197" t="s">
+      <c r="G24" s="174" t="s">
+        <v>115</v>
+      </c>
+      <c r="H24" s="191" t="s">
         <v>99</v>
       </c>
-      <c r="I24" s="198"/>
+      <c r="I24" s="192"/>
       <c r="J24" s="176"/>
     </row>
     <row r="25" spans="1:10" s="169" customFormat="1">
@@ -6217,14 +6223,14 @@
         <v>20</v>
       </c>
       <c r="C25" s="170"/>
-      <c r="D25" s="200"/>
+      <c r="D25" s="194"/>
       <c r="E25" s="175"/>
       <c r="F25" s="81"/>
       <c r="G25" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="H25" s="199"/>
-      <c r="I25" s="200"/>
+      <c r="H25" s="193"/>
+      <c r="I25" s="194"/>
       <c r="J25" s="176"/>
     </row>
     <row r="26" spans="1:10" s="169" customFormat="1">
@@ -6236,7 +6242,7 @@
         <v>62</v>
       </c>
       <c r="C26" s="170"/>
-      <c r="D26" s="206"/>
+      <c r="D26" s="200"/>
       <c r="E26" s="178" t="s">
         <v>103</v>
       </c>
@@ -6246,10 +6252,10 @@
       <c r="G26" s="174" t="s">
         <v>105</v>
       </c>
-      <c r="H26" s="197" t="s">
+      <c r="H26" s="191" t="s">
         <v>106</v>
       </c>
-      <c r="I26" s="198" t="s">
+      <c r="I26" s="192" t="s">
         <v>107</v>
       </c>
       <c r="J26" s="176"/>
@@ -6263,14 +6269,14 @@
         <v>20</v>
       </c>
       <c r="C27" s="170"/>
-      <c r="D27" s="200"/>
+      <c r="D27" s="194"/>
       <c r="E27" s="175"/>
       <c r="F27" s="81"/>
       <c r="G27" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="H27" s="199"/>
-      <c r="I27" s="200"/>
+      <c r="H27" s="193"/>
+      <c r="I27" s="194"/>
       <c r="J27" s="176"/>
     </row>
     <row r="28" spans="1:10" s="169" customFormat="1" ht="15" thickBot="1">
@@ -6282,16 +6288,16 @@
         <v>20</v>
       </c>
       <c r="C28" s="170"/>
-      <c r="D28" s="200"/>
+      <c r="D28" s="194"/>
       <c r="E28" s="179" t="s">
         <v>90</v>
       </c>
-      <c r="F28" s="201"/>
-      <c r="G28" s="202" t="s">
+      <c r="F28" s="195"/>
+      <c r="G28" s="196" t="s">
         <v>91</v>
       </c>
-      <c r="H28" s="203"/>
-      <c r="I28" s="204"/>
+      <c r="H28" s="197"/>
+      <c r="I28" s="198"/>
       <c r="J28" s="176"/>
     </row>
     <row r="29" spans="1:10" s="169" customFormat="1">
@@ -6304,22 +6310,22 @@
       </c>
       <c r="C29" s="173"/>
       <c r="D29" s="173"/>
-      <c r="E29" s="193" t="s">
+      <c r="E29" s="187" t="s">
         <v>111</v>
       </c>
-      <c r="F29" s="194" t="s">
+      <c r="F29" s="188" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="194" t="s">
+      <c r="G29" s="188" t="s">
         <v>4</v>
       </c>
-      <c r="H29" s="196" t="s">
+      <c r="H29" s="190" t="s">
         <v>4</v>
       </c>
-      <c r="I29" s="207" t="s">
+      <c r="I29" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="208"/>
+      <c r="J29" s="202"/>
     </row>
     <row r="30" spans="1:10" s="169" customFormat="1">
       <c r="A30" s="166">
@@ -6332,16 +6338,16 @@
       <c r="C30" s="168">
         <v>2</v>
       </c>
-      <c r="D30" s="205" t="s">
+      <c r="D30" s="199" t="s">
         <v>112</v>
       </c>
       <c r="E30" s="178" t="s">
         <v>98</v>
       </c>
-      <c r="F30" s="209"/>
-      <c r="G30" s="209"/>
+      <c r="F30" s="203"/>
+      <c r="G30" s="203"/>
       <c r="H30" s="177"/>
-      <c r="I30" s="210"/>
+      <c r="I30" s="204"/>
       <c r="J30" s="176"/>
     </row>
     <row r="31" spans="1:10" s="169" customFormat="1">
@@ -6356,13 +6362,13 @@
       <c r="D31" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="211" t="s">
+      <c r="E31" s="205" t="s">
         <v>90</v>
       </c>
-      <c r="F31" s="209"/>
-      <c r="G31" s="209"/>
-      <c r="H31" s="209"/>
-      <c r="I31" s="210"/>
+      <c r="F31" s="203"/>
+      <c r="G31" s="203"/>
+      <c r="H31" s="203"/>
+      <c r="I31" s="204"/>
       <c r="J31" s="176"/>
     </row>
     <row r="32" spans="1:10" s="169" customFormat="1" ht="15" thickBot="1">
@@ -6374,12 +6380,12 @@
         <v>20</v>
       </c>
       <c r="C32" s="180"/>
-      <c r="D32" s="202"/>
-      <c r="E32" s="212"/>
-      <c r="F32" s="213"/>
-      <c r="G32" s="213"/>
-      <c r="H32" s="213"/>
-      <c r="I32" s="214"/>
+      <c r="D32" s="196"/>
+      <c r="E32" s="206"/>
+      <c r="F32" s="207"/>
+      <c r="G32" s="207"/>
+      <c r="H32" s="207"/>
+      <c r="I32" s="208"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>